<commit_message>
adicionando uma pancada de coisa
</commit_message>
<xml_diff>
--- a/Catalog.xlsx
+++ b/Catalog.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="622">
   <si>
     <t xml:space="preserve">Ancient Middle-East</t>
   </si>
@@ -1882,6 +1882,9 @@
   </si>
   <si>
     <t>https://www.reddit.com/r/IcebergCharts/comments/w8cqi6/declassified_government_documents_iceberg/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Secret King: The Myth and Reality of Nazi Occultism</t>
   </si>
   <si>
     <t xml:space="preserve">A Critique of “Reason” Luke Smith</t>
@@ -50224,6 +50227,11 @@
     </row>
     <row r="22" ht="12.75"/>
     <row r="23" ht="12.75"/>
+    <row r="27" ht="12.75">
+      <c r="A27" t="s">
+        <v>620</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A21"/>
@@ -50242,14 +50250,14 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="46.140625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="61" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>